<commit_message>
chore(playground): update vue-demo to use simplified config
- Migrate from verbose config to defineConfig() pattern
- Remove ja-JP locale (reduce to zh-CN and en-US only)
- Update locale files with latest translations
- Demonstrate the new minimal configuration approach
</commit_message>
<xml_diff>
--- a/apps/playground/vue-demo/translations/translations.xlsx
+++ b/apps/playground/vue-demo/translations/translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13440"/>
+    <workbookView windowWidth="30240" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="80">
   <si>
     <t>Key</t>
   </si>
@@ -56,7 +56,7 @@
     <t>交互演示</t>
   </si>
   <si>
-    <t>interact</t>
+    <t>demo</t>
   </si>
   <si>
     <t>pending</t>
@@ -71,9 +71,6 @@
     <t>切换中...</t>
   </si>
   <si>
-    <t>switching...</t>
-  </si>
-  <si>
     <t>11134119</t>
   </si>
   <si>
@@ -176,18 +173,12 @@
     <t>加入时间</t>
   </si>
   <si>
-    <t>joinned time</t>
-  </si>
-  <si>
     <t>21511119</t>
   </si>
   <si>
     <t>当前语言</t>
   </si>
   <si>
-    <t>curretn lang</t>
-  </si>
-  <si>
     <t>31021111</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>消息通知</t>
   </si>
   <si>
-    <t>message notify</t>
-  </si>
-  <si>
     <t>42612454</t>
   </si>
   <si>
@@ -233,34 +221,22 @@
     <t>发布文章</t>
   </si>
   <si>
-    <t>publish article</t>
-  </si>
-  <si>
     <t>52134415</t>
   </si>
   <si>
     <t>高级用户</t>
   </si>
   <si>
-    <t>highly user</t>
-  </si>
-  <si>
     <t>61471412</t>
   </si>
   <si>
     <t>编辑资料</t>
   </si>
   <si>
-    <t>edit info</t>
-  </si>
-  <si>
     <t>71101173</t>
   </si>
   <si>
     <t>数据展示</t>
-  </si>
-  <si>
-    <t>database display</t>
   </si>
   <si>
     <t>71651251</t>
@@ -298,30 +274,30 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -329,7 +305,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -337,14 +313,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -352,7 +328,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -360,7 +336,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -368,7 +344,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -376,7 +352,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -384,14 +360,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -399,7 +375,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -407,7 +383,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -415,14 +391,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -430,42 +406,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -779,7 +755,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -788,7 +764,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -931,55 +907,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Link" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="Explanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1315,9 +1291,9 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
@@ -1381,7 +1357,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1398,10 +1374,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1421,10 +1397,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1444,10 +1420,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1467,10 +1443,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1490,13 +1466,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1513,13 +1489,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1536,10 +1512,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1559,10 +1535,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1582,10 +1558,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1605,10 +1581,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1628,10 +1604,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1651,10 +1627,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -1674,10 +1650,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1697,10 +1673,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1720,10 +1696,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1743,13 +1719,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -1766,13 +1742,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -1789,10 +1765,10 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1812,10 +1788,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1835,10 +1811,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1858,13 +1834,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
@@ -1881,10 +1857,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1904,10 +1880,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1927,13 +1903,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1950,13 +1926,13 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -1973,13 +1949,13 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -1996,13 +1972,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -2019,10 +1995,10 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
@@ -2042,10 +2018,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -2065,10 +2041,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -2088,10 +2064,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -2111,10 +2087,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>

</xml_diff>